<commit_message>
docs: v&v - traceability for system FRs
</commit_message>
<xml_diff>
--- a/docs/VnVPlan/traceability_tests_and_requirements.xlsx
+++ b/docs/VnVPlan/traceability_tests_and_requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcmasteru365-my.sharepoint.com/personal/wanga91_mcmaster_ca/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="8_{4056B838-B75A-4DB4-B350-64EB1252DAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F9805AE-9B9C-4DFF-9530-6D4A9DA85188}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="8_{4056B838-B75A-4DB4-B350-64EB1252DAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35A468AF-0D62-4161-9900-B7BD0C951F02}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="1" xr2:uid="{4EF2AD0A-3050-457B-B020-098845F115A5}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{4EF2AD0A-3050-457B-B020-098845F115A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional Requirements" sheetId="2" r:id="rId1"/>
@@ -37,11 +37,71 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="109">
   <si>
     <t>Test ID</t>
   </si>
   <si>
+    <t>FR1</t>
+  </si>
+  <si>
+    <t>FR2</t>
+  </si>
+  <si>
+    <t>FR3</t>
+  </si>
+  <si>
+    <t>FR4</t>
+  </si>
+  <si>
+    <t>FR5</t>
+  </si>
+  <si>
+    <t>FR6</t>
+  </si>
+  <si>
+    <t>FR7</t>
+  </si>
+  <si>
+    <t>FR8</t>
+  </si>
+  <si>
+    <t>FR9</t>
+  </si>
+  <si>
+    <t>FR10</t>
+  </si>
+  <si>
+    <t>FR11</t>
+  </si>
+  <si>
+    <t>FR12</t>
+  </si>
+  <si>
+    <t>FR13</t>
+  </si>
+  <si>
+    <t>FR14</t>
+  </si>
+  <si>
+    <t>FR15</t>
+  </si>
+  <si>
+    <t>FR16</t>
+  </si>
+  <si>
+    <t>FR17</t>
+  </si>
+  <si>
+    <t>FR18</t>
+  </si>
+  <si>
+    <t>FR19</t>
+  </si>
+  <si>
+    <t>FR20</t>
+  </si>
+  <si>
     <t>NFR1</t>
   </si>
   <si>
@@ -241,6 +301,69 @@
   </si>
   <si>
     <t>test-REG-1</t>
+  </si>
+  <si>
+    <t>test-UAM-1</t>
+  </si>
+  <si>
+    <t>test-UAM-2</t>
+  </si>
+  <si>
+    <t>test-UAM-3</t>
+  </si>
+  <si>
+    <t>test-UAM-4</t>
+  </si>
+  <si>
+    <t>test-IP-1</t>
+  </si>
+  <si>
+    <t>test-IP-2</t>
+  </si>
+  <si>
+    <t>test-UAM-5</t>
+  </si>
+  <si>
+    <t>test-UAM-6</t>
+  </si>
+  <si>
+    <t>test-IP-3</t>
+  </si>
+  <si>
+    <t>FR21</t>
+  </si>
+  <si>
+    <t>FR22</t>
+  </si>
+  <si>
+    <t>FR23</t>
+  </si>
+  <si>
+    <t>test-MIS-1</t>
+  </si>
+  <si>
+    <t>test-DM-1</t>
+  </si>
+  <si>
+    <t>test-DM-2</t>
+  </si>
+  <si>
+    <t>test-RS-1</t>
+  </si>
+  <si>
+    <t>test-RS-2</t>
+  </si>
+  <si>
+    <t>test-RS-3</t>
+  </si>
+  <si>
+    <t>test-FT-1</t>
+  </si>
+  <si>
+    <t>test-FT-2</t>
+  </si>
+  <si>
+    <t>test-FT-3</t>
   </si>
 </sst>
 </file>
@@ -362,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -378,6 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,12 +836,457 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A66D1D8B-B413-4D77-8ACB-D92046B60C6B}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:O22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="10"/>
+      <c r="M11" s="11"/>
+    </row>
+    <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="7"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M20" s="1"/>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="7"/>
+    </row>
+    <row r="22" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -726,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A06C17-E2CA-4A17-B084-FA5E0A852659}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,39 +1311,39 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -787,11 +1356,11 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -803,12 +1372,12 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -819,13 +1388,13 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -835,14 +1404,14 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -851,7 +1420,7 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -859,7 +1428,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -867,7 +1436,7 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -876,14 +1445,14 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -893,13 +1462,13 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -910,7 +1479,7 @@
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="11" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -929,42 +1498,42 @@
         <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -972,7 +1541,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -980,14 +1549,14 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -999,7 +1568,7 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1009,26 +1578,26 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="7"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1037,7 +1606,7 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="12" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1048,10 +1617,10 @@
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1087,46 +1656,46 @@
         <v>0</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="6" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1142,11 +1711,11 @@
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="6" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1161,12 +1730,12 @@
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="6" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1180,13 +1749,13 @@
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="8" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1199,17 +1768,17 @@
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="8" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1219,7 +1788,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1228,7 +1797,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1237,7 +1806,7 @@
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -1247,16 +1816,16 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
       <c r="J28" s="10" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="L28" s="13" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="M28" s="14" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1265,62 +1834,62 @@
         <v>0</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1328,12 +1897,12 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -1341,14 +1910,14 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="7"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1356,7 +1925,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1366,7 +1935,7 @@
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="9" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -1378,10 +1947,10 @@
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
       <c r="L34" s="10" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="M34" s="11" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>